<commit_message>
Ajuste de plantilla (v1.4.1)
</commit_message>
<xml_diff>
--- a/public/plantilla_sinapsis.xlsx
+++ b/public/plantilla_sinapsis.xlsx
@@ -772,9 +772,9 @@
   </sheetPr>
   <dimension ref="A1:CY1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CJ9" sqref="CJ9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1095,7 +1095,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>